<commit_message>
updating to list each job array number
</commit_message>
<xml_diff>
--- a/stochastic_storm_transposition/local/da_job_array_numbers.xlsx
+++ b/stochastic_storm_transposition/local/da_job_array_numbers.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\_GradSchool\_norfolk\stormy\stochastic_storm_transposition\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C45B6C8-B0EA-4E19-A459-A589478E7C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ECB30F-5A30-4CC7-870F-9A6C527D500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{75DFC11A-28C4-401C-8FA0-9737E100FF65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{75DFC11A-28C4-401C-8FA0-9737E100FF65}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="option 1" sheetId="1" r:id="rId1"/>
+    <sheet name="option 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>years</t>
   </si>
@@ -114,8 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D433A51A-3FC9-4E22-9B1E-71A313541299}">
   <dimension ref="B3:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,28 +450,28 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -545,7 +548,7 @@
         <v>20021</v>
       </c>
       <c r="J5" t="str">
-        <f>_xlfn.CONCAT($B5, H5)</f>
+        <f t="shared" ref="J5:J22" si="1">_xlfn.CONCAT($B5, H5)</f>
         <v>20026</v>
       </c>
       <c r="K5" t="str">
@@ -556,11 +559,11 @@
         <v>5</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5:M22" si="1">IF(L5="yes", ",", "")</f>
+        <f t="shared" ref="M5:M22" si="2">IF(L5="yes", ",", "")</f>
         <v>,</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N22" si="2">_xlfn.CONCAT(K5,M5)</f>
+        <f>_xlfn.CONCAT(K5,M5)</f>
         <v>20021-20026,</v>
       </c>
     </row>
@@ -591,7 +594,7 @@
         <v>20031</v>
       </c>
       <c r="J6" t="str">
-        <f>_xlfn.CONCAT($B6, H6)</f>
+        <f t="shared" si="1"/>
         <v>20036</v>
       </c>
       <c r="K6" t="str">
@@ -602,11 +605,11 @@
         <v>5</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K6,M6)</f>
         <v>20031-20036,</v>
       </c>
     </row>
@@ -637,7 +640,7 @@
         <v>20041</v>
       </c>
       <c r="J7" t="str">
-        <f>_xlfn.CONCAT($B7, H7)</f>
+        <f t="shared" si="1"/>
         <v>20046</v>
       </c>
       <c r="K7" t="str">
@@ -648,11 +651,11 @@
         <v>5</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K7,M7)</f>
         <v>20041-20046,</v>
       </c>
     </row>
@@ -683,7 +686,7 @@
         <v>20051</v>
       </c>
       <c r="J8" t="str">
-        <f>_xlfn.CONCAT($B8, H8)</f>
+        <f t="shared" si="1"/>
         <v>20056</v>
       </c>
       <c r="K8" t="str">
@@ -694,11 +697,11 @@
         <v>5</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K8,M8)</f>
         <v>20051-20056,</v>
       </c>
     </row>
@@ -729,7 +732,7 @@
         <v>20061</v>
       </c>
       <c r="J9" t="str">
-        <f>_xlfn.CONCAT($B9, H9)</f>
+        <f t="shared" si="1"/>
         <v>20066</v>
       </c>
       <c r="K9" t="str">
@@ -740,11 +743,11 @@
         <v>5</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K9,M9)</f>
         <v>20061-20066,</v>
       </c>
     </row>
@@ -775,7 +778,7 @@
         <v>20071</v>
       </c>
       <c r="J10" t="str">
-        <f>_xlfn.CONCAT($B10, H10)</f>
+        <f t="shared" si="1"/>
         <v>20076</v>
       </c>
       <c r="K10" t="str">
@@ -786,11 +789,11 @@
         <v>5</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K10,M10)</f>
         <v>20071-20076,</v>
       </c>
     </row>
@@ -821,7 +824,7 @@
         <v>20081</v>
       </c>
       <c r="J11" t="str">
-        <f>_xlfn.CONCAT($B11, H11)</f>
+        <f t="shared" si="1"/>
         <v>20086</v>
       </c>
       <c r="K11" t="str">
@@ -832,11 +835,11 @@
         <v>5</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K11,M11)</f>
         <v>20081-20086,</v>
       </c>
     </row>
@@ -867,7 +870,7 @@
         <v>20091</v>
       </c>
       <c r="J12" t="str">
-        <f>_xlfn.CONCAT($B12, H12)</f>
+        <f t="shared" si="1"/>
         <v>20096</v>
       </c>
       <c r="K12" t="str">
@@ -878,11 +881,11 @@
         <v>5</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K12,M12)</f>
         <v>20091-20096,</v>
       </c>
     </row>
@@ -913,7 +916,7 @@
         <v>20101</v>
       </c>
       <c r="J13" t="str">
-        <f>_xlfn.CONCAT($B13, H13)</f>
+        <f t="shared" si="1"/>
         <v>20106</v>
       </c>
       <c r="K13" t="str">
@@ -924,11 +927,11 @@
         <v>5</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K13,M13)</f>
         <v>20101-20106,</v>
       </c>
     </row>
@@ -959,7 +962,7 @@
         <v>20111</v>
       </c>
       <c r="J14" t="str">
-        <f>_xlfn.CONCAT($B14, H14)</f>
+        <f t="shared" si="1"/>
         <v>20116</v>
       </c>
       <c r="K14" t="str">
@@ -970,11 +973,11 @@
         <v>5</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K14,M14)</f>
         <v>20111-20116,</v>
       </c>
     </row>
@@ -1005,7 +1008,7 @@
         <v>20151</v>
       </c>
       <c r="J15" t="str">
-        <f>_xlfn.CONCAT($B15, H15)</f>
+        <f t="shared" si="1"/>
         <v>20156</v>
       </c>
       <c r="K15" t="str">
@@ -1016,11 +1019,11 @@
         <v>5</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K15,M15)</f>
         <v>20151-20156,</v>
       </c>
     </row>
@@ -1051,7 +1054,7 @@
         <v>20161</v>
       </c>
       <c r="J16" t="str">
-        <f>_xlfn.CONCAT($B16, H16)</f>
+        <f t="shared" si="1"/>
         <v>20166</v>
       </c>
       <c r="K16" t="str">
@@ -1062,11 +1065,11 @@
         <v>5</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K16,M16)</f>
         <v>20161-20166,</v>
       </c>
     </row>
@@ -1097,7 +1100,7 @@
         <v>20171</v>
       </c>
       <c r="J17" t="str">
-        <f>_xlfn.CONCAT($B17, H17)</f>
+        <f t="shared" si="1"/>
         <v>20176</v>
       </c>
       <c r="K17" t="str">
@@ -1108,11 +1111,11 @@
         <v>5</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K17,M17)</f>
         <v>20171-20176,</v>
       </c>
     </row>
@@ -1143,7 +1146,7 @@
         <v>20181</v>
       </c>
       <c r="J18" t="str">
-        <f>_xlfn.CONCAT($B18, H18)</f>
+        <f t="shared" si="1"/>
         <v>20186</v>
       </c>
       <c r="K18" t="str">
@@ -1154,11 +1157,11 @@
         <v>5</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K18,M18)</f>
         <v>20181-20186,</v>
       </c>
     </row>
@@ -1189,7 +1192,7 @@
         <v>20191</v>
       </c>
       <c r="J19" t="str">
-        <f>_xlfn.CONCAT($B19, H19)</f>
+        <f t="shared" si="1"/>
         <v>20196</v>
       </c>
       <c r="K19" t="str">
@@ -1200,11 +1203,11 @@
         <v>5</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K19,M19)</f>
         <v>20191-20196,</v>
       </c>
     </row>
@@ -1235,7 +1238,7 @@
         <v>20201</v>
       </c>
       <c r="J20" t="str">
-        <f>_xlfn.CONCAT($B20, H20)</f>
+        <f t="shared" si="1"/>
         <v>20206</v>
       </c>
       <c r="K20" t="str">
@@ -1246,11 +1249,11 @@
         <v>5</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K20,M20)</f>
         <v>20201-20206,</v>
       </c>
     </row>
@@ -1281,7 +1284,7 @@
         <v>20211</v>
       </c>
       <c r="J21" t="str">
-        <f>_xlfn.CONCAT($B21, H21)</f>
+        <f t="shared" si="1"/>
         <v>20216</v>
       </c>
       <c r="K21" t="str">
@@ -1292,11 +1295,11 @@
         <v>5</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K21,M21)</f>
         <v>20211-20216,</v>
       </c>
     </row>
@@ -1327,7 +1330,7 @@
         <v>20221</v>
       </c>
       <c r="J22" t="str">
-        <f>_xlfn.CONCAT($B22, H22)</f>
+        <f t="shared" si="1"/>
         <v>20226</v>
       </c>
       <c r="K22" t="str">
@@ -1338,21 +1341,976 @@
         <v>6</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(K22,M22)</f>
         <v>20221-20226</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" t="str">
         <f>_xlfn.CONCAT(N4:N22)</f>
         <v>20011-20016,20021-20026,20031-20036,20041-20046,20051-20056,20061-20066,20071-20076,20081-20086,20091-20096,20101-20106,20111-20116,20151-20156,20161-20166,20171-20176,20181-20186,20191-20196,20201-20206,20211-20216,20221-20226</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5200464E-82D5-403A-A7ED-59BE9B8394BF}">
+  <dimension ref="B3:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2001</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4" t="str">
+        <f>_xlfn.CONCAT($B4, C4, ",")</f>
+        <v>20011,</v>
+      </c>
+      <c r="J4" t="str">
+        <f>_xlfn.CONCAT($B4, D4, ",")</f>
+        <v>20012,</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" ref="K4:N19" si="0">_xlfn.CONCAT($B4, E4, ",")</f>
+        <v>20013,</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>20014,</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>20015,</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>20016,</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2002</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" ref="I5:N22" si="1">_xlfn.CONCAT($B5, C5, ",")</f>
+        <v>20021,</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>20022,</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>20023,</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>20024,</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>20025,</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>20026,</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2003</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>20031,</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>20032,</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>20033,</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>20034,</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>20035,</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>20036,</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>2004</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>20041,</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>20042,</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>20043,</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>20044,</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>20045,</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>20046,</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2005</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>20051,</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>20052,</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>20053,</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>20054,</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>20055,</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>20056,</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2006</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>20061,</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>20062,</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>20063,</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>20064,</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>20065,</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>20066,</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2007</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>20071,</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>20072,</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>20073,</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>20074,</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>20075,</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>20076,</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2008</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>20081,</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>20082,</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>20083,</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>20084,</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>20085,</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>20086,</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2009</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>20091,</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>20092,</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>20093,</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>20094,</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>20095,</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>20096,</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2010</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>20101,</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>20102,</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>20103,</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>20104,</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>20105,</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>20106,</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2011</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>20111,</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>20112,</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>20113,</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>20114,</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>20115,</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>20116,</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2015</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>20151,</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>20152,</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>20153,</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>20154,</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>20155,</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>20156,</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2016</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>20161,</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>20162,</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>20163,</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>20164,</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>20165,</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>20166,</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2017</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>20171,</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>20172,</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>20173,</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>20174,</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>20175,</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>20176,</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2018</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>6</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>20181,</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>20182,</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>20183,</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>20184,</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>20185,</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>20186,</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2019</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>20191,</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>20192,</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>20193,</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>20194,</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>20195,</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>20196,</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2020</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>20201,</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>20202,</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>20203,</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>20204,</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>20205,</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>20206,</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2021</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>6</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>20211,</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>20212,</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="1"/>
+        <v>20213,</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>20214,</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>20215,</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>20216,</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>20221,</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>20222,</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="1"/>
+        <v>20223,</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>20224,</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="1"/>
+        <v>20225,</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="1"/>
+        <v>20226,</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D26" s="2"/>
+      <c r="E26" t="str">
+        <f>_xlfn.CONCAT(R4:R22)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="str">
+        <f>_xlfn.CONCAT(I4:N22)</f>
+        <v>20011,20012,20013,20014,20015,20016,20021,20022,20023,20024,20025,20026,20031,20032,20033,20034,20035,20036,20041,20042,20043,20044,20045,20046,20051,20052,20053,20054,20055,20056,20061,20062,20063,20064,20065,20066,20071,20072,20073,20074,20075,20076,20081,20082,20083,20084,20085,20086,20091,20092,20093,20094,20095,20096,20101,20102,20103,20104,20105,20106,20111,20112,20113,20114,20115,20116,20151,20152,20153,20154,20155,20156,20161,20162,20163,20164,20165,20166,20171,20172,20173,20174,20175,20176,20181,20182,20183,20184,20185,20186,20191,20192,20193,20194,20195,20196,20201,20202,20203,20204,20205,20206,20211,20212,20213,20214,20215,20216,20221,20222,20223,20224,20225,20226,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing so that the job nums were less than 1000
</commit_message>
<xml_diff>
--- a/stochastic_storm_transposition/local/da_job_array_numbers.xlsx
+++ b/stochastic_storm_transposition/local/da_job_array_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\_GradSchool\_norfolk\stormy\stochastic_storm_transposition\local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ECB30F-5A30-4CC7-870F-9A6C527D500E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D08AAF-E1F1-42AD-BEAC-40837335FBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{75DFC11A-28C4-401C-8FA0-9737E100FF65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{75DFC11A-28C4-401C-8FA0-9737E100FF65}"/>
   </bookViews>
   <sheets>
     <sheet name="option 1" sheetId="1" r:id="rId1"/>
@@ -435,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D433A51A-3FC9-4E22-9B1E-71A313541299}">
   <dimension ref="B3:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>2001</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -499,15 +499,15 @@
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT($B4, C4)</f>
-        <v>20011</v>
+        <v>11</v>
       </c>
       <c r="J4" t="str">
         <f>_xlfn.CONCAT($B4, H4)</f>
-        <v>20016</v>
+        <v>16</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.CONCAT(I4, "-", J4)</f>
-        <v>20011-20016</v>
+        <f t="shared" ref="K4:K22" si="0">_xlfn.CONCAT(I4, "-", J4)</f>
+        <v>11-16</v>
       </c>
       <c r="L4" t="s">
         <v>5</v>
@@ -517,13 +517,13 @@
         <v>,</v>
       </c>
       <c r="N4" t="str">
-        <f>_xlfn.CONCAT(K4,M4)</f>
-        <v>20011-20016,</v>
+        <f t="shared" ref="N4:N22" si="1">_xlfn.CONCAT(K4,M4)</f>
+        <v>11-16,</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>2002</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -544,32 +544,32 @@
         <v>6</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" ref="I5:I22" si="0">_xlfn.CONCAT($B5, C5)</f>
-        <v>20021</v>
+        <f t="shared" ref="I5:I22" si="2">_xlfn.CONCAT($B5, C5)</f>
+        <v>21</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ref="J5:J22" si="1">_xlfn.CONCAT($B5, H5)</f>
-        <v>20026</v>
+        <f t="shared" ref="J5:J22" si="3">_xlfn.CONCAT($B5, H5)</f>
+        <v>26</v>
       </c>
       <c r="K5" t="str">
-        <f>_xlfn.CONCAT(I5, "-", J5)</f>
-        <v>20021-20026</v>
+        <f t="shared" si="0"/>
+        <v>21-26</v>
       </c>
       <c r="L5" t="s">
         <v>5</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" ref="M5:M22" si="2">IF(L5="yes", ",", "")</f>
+        <f t="shared" ref="M5:M22" si="4">IF(L5="yes", ",", "")</f>
         <v>,</v>
       </c>
       <c r="N5" t="str">
-        <f>_xlfn.CONCAT(K5,M5)</f>
-        <v>20021-20026,</v>
+        <f t="shared" si="1"/>
+        <v>21-26,</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>2003</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -590,32 +590,32 @@
         <v>6</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>20031</v>
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="1"/>
-        <v>20036</v>
+        <f t="shared" si="3"/>
+        <v>36</v>
       </c>
       <c r="K6" t="str">
-        <f>_xlfn.CONCAT(I6, "-", J6)</f>
-        <v>20031-20036</v>
+        <f t="shared" si="0"/>
+        <v>31-36</v>
       </c>
       <c r="L6" t="s">
         <v>5</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N6" t="str">
-        <f>_xlfn.CONCAT(K6,M6)</f>
-        <v>20031-20036,</v>
+        <f t="shared" si="1"/>
+        <v>31-36,</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>2004</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -636,32 +636,32 @@
         <v>6</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>20041</v>
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="1"/>
-        <v>20046</v>
+        <f t="shared" si="3"/>
+        <v>46</v>
       </c>
       <c r="K7" t="str">
-        <f>_xlfn.CONCAT(I7, "-", J7)</f>
-        <v>20041-20046</v>
+        <f t="shared" si="0"/>
+        <v>41-46</v>
       </c>
       <c r="L7" t="s">
         <v>5</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N7" t="str">
-        <f>_xlfn.CONCAT(K7,M7)</f>
-        <v>20041-20046,</v>
+        <f t="shared" si="1"/>
+        <v>41-46,</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>2005</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -682,32 +682,32 @@
         <v>6</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>20051</v>
+        <f t="shared" si="2"/>
+        <v>51</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="1"/>
-        <v>20056</v>
+        <f t="shared" si="3"/>
+        <v>56</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.CONCAT(I8, "-", J8)</f>
-        <v>20051-20056</v>
+        <f t="shared" si="0"/>
+        <v>51-56</v>
       </c>
       <c r="L8" t="s">
         <v>5</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N8" t="str">
-        <f>_xlfn.CONCAT(K8,M8)</f>
-        <v>20051-20056,</v>
+        <f t="shared" si="1"/>
+        <v>51-56,</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>2006</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -728,32 +728,32 @@
         <v>6</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>20061</v>
+        <f t="shared" si="2"/>
+        <v>61</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="1"/>
-        <v>20066</v>
+        <f t="shared" si="3"/>
+        <v>66</v>
       </c>
       <c r="K9" t="str">
-        <f>_xlfn.CONCAT(I9, "-", J9)</f>
-        <v>20061-20066</v>
+        <f t="shared" si="0"/>
+        <v>61-66</v>
       </c>
       <c r="L9" t="s">
         <v>5</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N9" t="str">
-        <f>_xlfn.CONCAT(K9,M9)</f>
-        <v>20061-20066,</v>
+        <f t="shared" si="1"/>
+        <v>61-66,</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>2007</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -774,32 +774,32 @@
         <v>6</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>20071</v>
+        <f t="shared" si="2"/>
+        <v>71</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="1"/>
-        <v>20076</v>
+        <f t="shared" si="3"/>
+        <v>76</v>
       </c>
       <c r="K10" t="str">
-        <f>_xlfn.CONCAT(I10, "-", J10)</f>
-        <v>20071-20076</v>
+        <f t="shared" si="0"/>
+        <v>71-76</v>
       </c>
       <c r="L10" t="s">
         <v>5</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N10" t="str">
-        <f>_xlfn.CONCAT(K10,M10)</f>
-        <v>20071-20076,</v>
+        <f t="shared" si="1"/>
+        <v>71-76,</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>2008</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -820,32 +820,32 @@
         <v>6</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>20081</v>
+        <f t="shared" si="2"/>
+        <v>81</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="1"/>
-        <v>20086</v>
+        <f t="shared" si="3"/>
+        <v>86</v>
       </c>
       <c r="K11" t="str">
-        <f>_xlfn.CONCAT(I11, "-", J11)</f>
-        <v>20081-20086</v>
+        <f t="shared" si="0"/>
+        <v>81-86</v>
       </c>
       <c r="L11" t="s">
         <v>5</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N11" t="str">
-        <f>_xlfn.CONCAT(K11,M11)</f>
-        <v>20081-20086,</v>
+        <f t="shared" si="1"/>
+        <v>81-86,</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>2009</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -866,32 +866,32 @@
         <v>6</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>20091</v>
+        <f t="shared" si="2"/>
+        <v>91</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="1"/>
-        <v>20096</v>
+        <f t="shared" si="3"/>
+        <v>96</v>
       </c>
       <c r="K12" t="str">
-        <f>_xlfn.CONCAT(I12, "-", J12)</f>
-        <v>20091-20096</v>
+        <f t="shared" si="0"/>
+        <v>91-96</v>
       </c>
       <c r="L12" t="s">
         <v>5</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N12" t="str">
-        <f>_xlfn.CONCAT(K12,M12)</f>
-        <v>20091-20096,</v>
+        <f t="shared" si="1"/>
+        <v>91-96,</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>2010</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -912,32 +912,32 @@
         <v>6</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>20101</v>
+        <f t="shared" si="2"/>
+        <v>101</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="1"/>
-        <v>20106</v>
+        <f t="shared" si="3"/>
+        <v>106</v>
       </c>
       <c r="K13" t="str">
-        <f>_xlfn.CONCAT(I13, "-", J13)</f>
-        <v>20101-20106</v>
+        <f t="shared" si="0"/>
+        <v>101-106</v>
       </c>
       <c r="L13" t="s">
         <v>5</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N13" t="str">
-        <f>_xlfn.CONCAT(K13,M13)</f>
-        <v>20101-20106,</v>
+        <f t="shared" si="1"/>
+        <v>101-106,</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>2011</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -958,32 +958,32 @@
         <v>6</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>20111</v>
+        <f t="shared" si="2"/>
+        <v>111</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="1"/>
-        <v>20116</v>
+        <f t="shared" si="3"/>
+        <v>116</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.CONCAT(I14, "-", J14)</f>
-        <v>20111-20116</v>
+        <f t="shared" si="0"/>
+        <v>111-116</v>
       </c>
       <c r="L14" t="s">
         <v>5</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N14" t="str">
-        <f>_xlfn.CONCAT(K14,M14)</f>
-        <v>20111-20116,</v>
+        <f t="shared" si="1"/>
+        <v>111-116,</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>2015</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1004,32 +1004,32 @@
         <v>6</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>20151</v>
+        <f t="shared" si="2"/>
+        <v>151</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="1"/>
-        <v>20156</v>
+        <f t="shared" si="3"/>
+        <v>156</v>
       </c>
       <c r="K15" t="str">
-        <f>_xlfn.CONCAT(I15, "-", J15)</f>
-        <v>20151-20156</v>
+        <f t="shared" si="0"/>
+        <v>151-156</v>
       </c>
       <c r="L15" t="s">
         <v>5</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N15" t="str">
-        <f>_xlfn.CONCAT(K15,M15)</f>
-        <v>20151-20156,</v>
+        <f t="shared" si="1"/>
+        <v>151-156,</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>2016</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1050,32 +1050,32 @@
         <v>6</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>20161</v>
+        <f t="shared" si="2"/>
+        <v>161</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="1"/>
-        <v>20166</v>
+        <f t="shared" si="3"/>
+        <v>166</v>
       </c>
       <c r="K16" t="str">
-        <f>_xlfn.CONCAT(I16, "-", J16)</f>
-        <v>20161-20166</v>
+        <f t="shared" si="0"/>
+        <v>161-166</v>
       </c>
       <c r="L16" t="s">
         <v>5</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N16" t="str">
-        <f>_xlfn.CONCAT(K16,M16)</f>
-        <v>20161-20166,</v>
+        <f t="shared" si="1"/>
+        <v>161-166,</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>2017</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1096,32 +1096,32 @@
         <v>6</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="0"/>
-        <v>20171</v>
+        <f t="shared" si="2"/>
+        <v>171</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="1"/>
-        <v>20176</v>
+        <f t="shared" si="3"/>
+        <v>176</v>
       </c>
       <c r="K17" t="str">
-        <f>_xlfn.CONCAT(I17, "-", J17)</f>
-        <v>20171-20176</v>
+        <f t="shared" si="0"/>
+        <v>171-176</v>
       </c>
       <c r="L17" t="s">
         <v>5</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N17" t="str">
-        <f>_xlfn.CONCAT(K17,M17)</f>
-        <v>20171-20176,</v>
+        <f t="shared" si="1"/>
+        <v>171-176,</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2018</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1142,32 +1142,32 @@
         <v>6</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>20181</v>
+        <f t="shared" si="2"/>
+        <v>181</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="1"/>
-        <v>20186</v>
+        <f t="shared" si="3"/>
+        <v>186</v>
       </c>
       <c r="K18" t="str">
-        <f>_xlfn.CONCAT(I18, "-", J18)</f>
-        <v>20181-20186</v>
+        <f t="shared" si="0"/>
+        <v>181-186</v>
       </c>
       <c r="L18" t="s">
         <v>5</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N18" t="str">
-        <f>_xlfn.CONCAT(K18,M18)</f>
-        <v>20181-20186,</v>
+        <f t="shared" si="1"/>
+        <v>181-186,</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>2019</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1188,32 +1188,32 @@
         <v>6</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>20191</v>
+        <f t="shared" si="2"/>
+        <v>191</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="1"/>
-        <v>20196</v>
+        <f t="shared" si="3"/>
+        <v>196</v>
       </c>
       <c r="K19" t="str">
-        <f>_xlfn.CONCAT(I19, "-", J19)</f>
-        <v>20191-20196</v>
+        <f t="shared" si="0"/>
+        <v>191-196</v>
       </c>
       <c r="L19" t="s">
         <v>5</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N19" t="str">
-        <f>_xlfn.CONCAT(K19,M19)</f>
-        <v>20191-20196,</v>
+        <f t="shared" si="1"/>
+        <v>191-196,</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>2020</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1234,32 +1234,32 @@
         <v>6</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>20201</v>
+        <f t="shared" si="2"/>
+        <v>201</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="1"/>
-        <v>20206</v>
+        <f t="shared" si="3"/>
+        <v>206</v>
       </c>
       <c r="K20" t="str">
-        <f>_xlfn.CONCAT(I20, "-", J20)</f>
-        <v>20201-20206</v>
+        <f t="shared" si="0"/>
+        <v>201-206</v>
       </c>
       <c r="L20" t="s">
         <v>5</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N20" t="str">
-        <f>_xlfn.CONCAT(K20,M20)</f>
-        <v>20201-20206,</v>
+        <f t="shared" si="1"/>
+        <v>201-206,</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>2021</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1280,32 +1280,32 @@
         <v>6</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>20211</v>
+        <f t="shared" si="2"/>
+        <v>211</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="1"/>
-        <v>20216</v>
+        <f t="shared" si="3"/>
+        <v>216</v>
       </c>
       <c r="K21" t="str">
-        <f>_xlfn.CONCAT(I21, "-", J21)</f>
-        <v>20211-20216</v>
+        <f t="shared" si="0"/>
+        <v>211-216</v>
       </c>
       <c r="L21" t="s">
         <v>5</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N21" t="str">
-        <f>_xlfn.CONCAT(K21,M21)</f>
-        <v>20211-20216,</v>
+        <f t="shared" si="1"/>
+        <v>211-216,</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>2022</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1326,27 +1326,27 @@
         <v>6</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>20221</v>
+        <f t="shared" si="2"/>
+        <v>221</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="1"/>
-        <v>20226</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="K22" t="str">
-        <f>_xlfn.CONCAT(I22, "-", J22)</f>
-        <v>20221-20226</v>
+        <f t="shared" si="0"/>
+        <v>221-226</v>
       </c>
       <c r="L22" t="s">
         <v>6</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="N22" t="str">
-        <f>_xlfn.CONCAT(K22,M22)</f>
-        <v>20221-20226</v>
+        <f t="shared" si="1"/>
+        <v>221-226</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="E26" t="str">
         <f>_xlfn.CONCAT(N4:N22)</f>
-        <v>20011-20016,20021-20026,20031-20036,20041-20046,20051-20056,20061-20066,20071-20076,20081-20086,20091-20096,20101-20106,20111-20116,20151-20156,20161-20166,20171-20176,20181-20186,20191-20196,20201-20206,20211-20216,20221-20226</v>
+        <v>11-16,21-26,31-36,41-46,51-56,61-66,71-76,81-86,91-96,101-106,111-116,151-156,161-166,171-176,181-186,191-196,201-206,211-216,221-226</v>
       </c>
     </row>
   </sheetData>
@@ -1372,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5200464E-82D5-403A-A7ED-59BE9B8394BF}">
   <dimension ref="B3:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>2001</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1428,32 +1428,32 @@
       </c>
       <c r="I4" t="str">
         <f>_xlfn.CONCAT($B4, C4, ",")</f>
-        <v>20011,</v>
+        <v>11,</v>
       </c>
       <c r="J4" t="str">
         <f>_xlfn.CONCAT($B4, D4, ",")</f>
-        <v>20012,</v>
+        <v>12,</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" ref="K4:N19" si="0">_xlfn.CONCAT($B4, E4, ",")</f>
-        <v>20013,</v>
+        <v>13,</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
-        <v>20014,</v>
+        <v>14,</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" si="0"/>
-        <v>20015,</v>
+        <v>15,</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" si="0"/>
-        <v>20016,</v>
+        <v>16,</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>2002</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1475,32 +1475,32 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" ref="I5:N22" si="1">_xlfn.CONCAT($B5, C5, ",")</f>
-        <v>20021,</v>
+        <v>21,</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
-        <v>20022,</v>
+        <v>22,</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
-        <v>20023,</v>
+        <v>23,</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
-        <v>20024,</v>
+        <v>24,</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="0"/>
-        <v>20025,</v>
+        <v>25,</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
-        <v>20026,</v>
+        <v>26,</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>2003</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1522,32 +1522,32 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>20031,</v>
+        <v>31,</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
-        <v>20032,</v>
+        <v>32,</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>20033,</v>
+        <v>33,</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
-        <v>20034,</v>
+        <v>34,</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="0"/>
-        <v>20035,</v>
+        <v>35,</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
-        <v>20036,</v>
+        <v>36,</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>2004</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1569,32 +1569,32 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>20041,</v>
+        <v>41,</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
-        <v>20042,</v>
+        <v>42,</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>20043,</v>
+        <v>43,</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
-        <v>20044,</v>
+        <v>44,</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="0"/>
-        <v>20045,</v>
+        <v>45,</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
-        <v>20046,</v>
+        <v>46,</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>2005</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1616,32 +1616,32 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>20051,</v>
+        <v>51,</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
-        <v>20052,</v>
+        <v>52,</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>20053,</v>
+        <v>53,</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="0"/>
-        <v>20054,</v>
+        <v>54,</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="0"/>
-        <v>20055,</v>
+        <v>55,</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
-        <v>20056,</v>
+        <v>56,</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>2006</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1663,32 +1663,32 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>20061,</v>
+        <v>61,</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
-        <v>20062,</v>
+        <v>62,</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>20063,</v>
+        <v>63,</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="0"/>
-        <v>20064,</v>
+        <v>64,</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="0"/>
-        <v>20065,</v>
+        <v>65,</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
-        <v>20066,</v>
+        <v>66,</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>2007</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1710,32 +1710,32 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>20071,</v>
+        <v>71,</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v>20072,</v>
+        <v>72,</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>20073,</v>
+        <v>73,</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="0"/>
-        <v>20074,</v>
+        <v>74,</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="0"/>
-        <v>20075,</v>
+        <v>75,</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
-        <v>20076,</v>
+        <v>76,</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>2008</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1757,32 +1757,32 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>20081,</v>
+        <v>81,</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
-        <v>20082,</v>
+        <v>82,</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>20083,</v>
+        <v>83,</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="0"/>
-        <v>20084,</v>
+        <v>84,</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="0"/>
-        <v>20085,</v>
+        <v>85,</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
-        <v>20086,</v>
+        <v>86,</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>2009</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1804,32 +1804,32 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
-        <v>20091,</v>
+        <v>91,</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="1"/>
-        <v>20092,</v>
+        <v>92,</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>20093,</v>
+        <v>93,</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="0"/>
-        <v>20094,</v>
+        <v>94,</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="0"/>
-        <v>20095,</v>
+        <v>95,</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
-        <v>20096,</v>
+        <v>96,</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>2010</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1851,32 +1851,32 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>20101,</v>
+        <v>101,</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
-        <v>20102,</v>
+        <v>102,</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>20103,</v>
+        <v>103,</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="0"/>
-        <v>20104,</v>
+        <v>104,</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="0"/>
-        <v>20105,</v>
+        <v>105,</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
-        <v>20106,</v>
+        <v>106,</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>2011</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1898,32 +1898,32 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
-        <v>20111,</v>
+        <v>111,</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="1"/>
-        <v>20112,</v>
+        <v>112,</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>20113,</v>
+        <v>113,</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="0"/>
-        <v>20114,</v>
+        <v>114,</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="0"/>
-        <v>20115,</v>
+        <v>115,</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
-        <v>20116,</v>
+        <v>116,</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
-        <v>2015</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1945,32 +1945,32 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
-        <v>20151,</v>
+        <v>151,</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="1"/>
-        <v>20152,</v>
+        <v>152,</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>20153,</v>
+        <v>153,</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="0"/>
-        <v>20154,</v>
+        <v>154,</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="0"/>
-        <v>20155,</v>
+        <v>155,</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
-        <v>20156,</v>
+        <v>156,</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>2016</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1992,32 +1992,32 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
-        <v>20161,</v>
+        <v>161,</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="1"/>
-        <v>20162,</v>
+        <v>162,</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>20163,</v>
+        <v>163,</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="0"/>
-        <v>20164,</v>
+        <v>164,</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="0"/>
-        <v>20165,</v>
+        <v>165,</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
-        <v>20166,</v>
+        <v>166,</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>2017</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2039,32 +2039,32 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>20171,</v>
+        <v>171,</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
-        <v>20172,</v>
+        <v>172,</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
-        <v>20173,</v>
+        <v>173,</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="0"/>
-        <v>20174,</v>
+        <v>174,</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="0"/>
-        <v>20175,</v>
+        <v>175,</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
-        <v>20176,</v>
+        <v>176,</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2018</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2086,32 +2086,32 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>20181,</v>
+        <v>181,</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
-        <v>20182,</v>
+        <v>182,</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
-        <v>20183,</v>
+        <v>183,</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="0"/>
-        <v>20184,</v>
+        <v>184,</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="0"/>
-        <v>20185,</v>
+        <v>185,</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
-        <v>20186,</v>
+        <v>186,</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>2019</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2133,32 +2133,32 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>20191,</v>
+        <v>191,</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
-        <v>20192,</v>
+        <v>192,</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v>20193,</v>
+        <v>193,</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="0"/>
-        <v>20194,</v>
+        <v>194,</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="0"/>
-        <v>20195,</v>
+        <v>195,</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="0"/>
-        <v>20196,</v>
+        <v>196,</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>2020</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2180,32 +2180,32 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>20201,</v>
+        <v>201,</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
-        <v>20202,</v>
+        <v>202,</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>20203,</v>
+        <v>203,</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="1"/>
-        <v>20204,</v>
+        <v>204,</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="1"/>
-        <v>20205,</v>
+        <v>205,</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="1"/>
-        <v>20206,</v>
+        <v>206,</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>2021</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2227,32 +2227,32 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>20211,</v>
+        <v>211,</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="1"/>
-        <v>20212,</v>
+        <v>212,</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>20213,</v>
+        <v>213,</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="1"/>
-        <v>20214,</v>
+        <v>214,</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="1"/>
-        <v>20215,</v>
+        <v>215,</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="1"/>
-        <v>20216,</v>
+        <v>216,</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>2022</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2274,27 +2274,27 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>20221,</v>
+        <v>221,</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="1"/>
-        <v>20222,</v>
+        <v>222,</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>20223,</v>
+        <v>223,</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="1"/>
-        <v>20224,</v>
+        <v>224,</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="1"/>
-        <v>20225,</v>
+        <v>225,</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="1"/>
-        <v>20226,</v>
+        <v>226,</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="C27" t="str">
         <f>_xlfn.CONCAT(I4:N22)</f>
-        <v>20011,20012,20013,20014,20015,20016,20021,20022,20023,20024,20025,20026,20031,20032,20033,20034,20035,20036,20041,20042,20043,20044,20045,20046,20051,20052,20053,20054,20055,20056,20061,20062,20063,20064,20065,20066,20071,20072,20073,20074,20075,20076,20081,20082,20083,20084,20085,20086,20091,20092,20093,20094,20095,20096,20101,20102,20103,20104,20105,20106,20111,20112,20113,20114,20115,20116,20151,20152,20153,20154,20155,20156,20161,20162,20163,20164,20165,20166,20171,20172,20173,20174,20175,20176,20181,20182,20183,20184,20185,20186,20191,20192,20193,20194,20195,20196,20201,20202,20203,20204,20205,20206,20211,20212,20213,20214,20215,20216,20221,20222,20223,20224,20225,20226,</v>
+        <v>11,12,13,14,15,16,21,22,23,24,25,26,31,32,33,34,35,36,41,42,43,44,45,46,51,52,53,54,55,56,61,62,63,64,65,66,71,72,73,74,75,76,81,82,83,84,85,86,91,92,93,94,95,96,101,102,103,104,105,106,111,112,113,114,115,116,151,152,153,154,155,156,161,162,163,164,165,166,171,172,173,174,175,176,181,182,183,184,185,186,191,192,193,194,195,196,201,202,203,204,205,206,211,212,213,214,215,216,221,222,223,224,225,226,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>